<commit_message>
Update to paper and excel with misclass rates
</commit_message>
<xml_diff>
--- a/Assignment Documents in Work/Boosted Tree Tuning Table and Validation Trials - Eric.xlsx
+++ b/Assignment Documents in Work/Boosted Tree Tuning Table and Validation Trials - Eric.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Documents\Villanova\Data Mining\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wezde\Documents\GitHub\MSA-8220_Final_Project\Assignment Documents in Work\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="6330" windowHeight="7185"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="6336" windowHeight="7188" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hypercubes" sheetId="1" r:id="rId1"/>
     <sheet name="Colinearity" sheetId="2" r:id="rId2"/>
     <sheet name="Alt Cutoff" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -193,11 +193,18 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -255,57 +262,64 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -621,455 +635,455 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
-    <col min="2" max="2" width="13" style="9" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.140625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" style="15" customWidth="1"/>
+    <col min="2" max="2" width="13" style="14" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.44140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.5546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.109375" style="14" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="13"/>
-    </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="13"/>
-    </row>
-    <row r="3" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="L1" s="7"/>
+    </row>
+    <row r="2" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="7"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="K3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="14"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="17">
         <v>5</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="7">
+      <c r="J4" s="17">
         <v>100</v>
       </c>
-      <c r="K4" s="11">
+      <c r="K4" s="18">
         <v>0.17280000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="17">
         <v>3</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="17">
         <v>5</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="7">
+      <c r="J5" s="17">
         <v>100</v>
       </c>
-      <c r="K5" s="11">
+      <c r="K5" s="18">
         <v>0.17380000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="17">
         <v>5</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6" s="17">
         <v>100</v>
       </c>
-      <c r="K6" s="11">
+      <c r="K6" s="18">
         <v>0.17449999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="17">
         <v>4</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="17">
         <v>5</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J7" s="17">
         <v>150</v>
       </c>
-      <c r="K7" s="11">
+      <c r="K7" s="18">
         <v>0.17030000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="15"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="B9" s="5"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="17" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="17">
         <v>3</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="17">
         <v>602020</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="17">
         <v>0.17380000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="17">
         <v>3</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="17">
         <v>403030</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="17">
         <v>0.17610000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="17">
         <v>3</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="17">
         <v>0.17380000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="7">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="17">
         <v>3</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="17">
         <v>0.17610000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="7">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="17">
         <v>3</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="17">
         <v>404020</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="17">
         <v>0.17119999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="7">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="17">
         <v>3</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="17">
         <v>305020</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="17">
         <v>0.17599999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="7">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="17">
         <v>3</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="17">
         <v>0.17219999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="17">
         <v>4</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18" s="17">
         <v>403030</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="17">
         <v>0.1774</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="7">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="17">
         <v>4</v>
       </c>
-      <c r="B19" s="7">
+      <c r="B19" s="17">
         <v>404020</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="17">
         <v>0.17130000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="19">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="20">
         <v>4</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C20" s="21">
         <v>0.17030000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="5"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="15" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="15" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="21" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="9">
+      <c r="B24" s="14">
         <v>602020</v>
       </c>
-      <c r="C24" s="9">
+      <c r="C24" s="14">
         <v>0.16170000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="21" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="9">
+      <c r="C25" s="14">
         <v>0.1767</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="9">
+      <c r="B26" s="14">
         <v>602020</v>
       </c>
-      <c r="C26" s="9">
+      <c r="C26" s="14">
         <v>0.1633</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="9">
+      <c r="B27" s="14">
         <v>602020</v>
       </c>
-      <c r="C27" s="9">
+      <c r="C27" s="14">
         <v>0.18129999999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="9">
+      <c r="B28" s="14">
         <v>602020</v>
       </c>
-      <c r="C28" s="9">
+      <c r="C28" s="14">
         <v>0.17299999999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="9">
+      <c r="C29" s="14">
         <v>0.17630000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="15" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C32" s="9">
+      <c r="C32" s="14">
         <v>0.1837</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="B33" s="9">
+      <c r="B33" s="14">
         <v>602020</v>
       </c>
-      <c r="C33" s="9">
+      <c r="C33" s="14">
         <v>0.16800000000000001</v>
       </c>
     </row>
@@ -1079,73 +1093,73 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="1">
         <v>0.17219999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="1">
         <v>0.17269999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="1">
         <v>0.17249999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="1">
         <v>0.17249999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="1">
         <v>0.17219999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="1">
         <v>0.17680000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="1">
         <v>0.17699999999999999</v>
       </c>
     </row>
@@ -1155,272 +1169,406 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="13.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="B3" s="2">
+        <v>4410</v>
+      </c>
+      <c r="C3" s="2">
+        <v>442</v>
+      </c>
+      <c r="D3" s="2">
+        <v>622</v>
+      </c>
+      <c r="E3" s="2">
+        <v>524</v>
+      </c>
+      <c r="F3" s="24">
+        <f>(C3+D3)/SUM(B3:E3)</f>
+        <v>0.17739246415471824</v>
+      </c>
+      <c r="G3" s="23">
+        <f>E3/SUM(B3:E3)</f>
+        <v>8.73624541513838E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>0.41</v>
+      </c>
+      <c r="B4" s="2">
+        <v>4438</v>
+      </c>
+      <c r="C4" s="2">
+        <v>414</v>
+      </c>
+      <c r="D4" s="2">
+        <v>636</v>
+      </c>
+      <c r="E4" s="2">
+        <v>512</v>
+      </c>
+      <c r="F4" s="24">
+        <f t="shared" ref="F4:F23" si="0">(C4+D4)/SUM(B4:E4)</f>
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="G4" s="23">
+        <f t="shared" ref="G4:G13" si="1">E4/SUM(B4:E4)</f>
+        <v>8.533333333333333E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>0.42</v>
+      </c>
+      <c r="B5" s="2">
+        <v>4461</v>
+      </c>
+      <c r="C5" s="2">
+        <v>391</v>
+      </c>
+      <c r="D5" s="2">
+        <v>648</v>
+      </c>
+      <c r="E5" s="2">
+        <v>500</v>
+      </c>
+      <c r="F5" s="24">
+        <f t="shared" si="0"/>
+        <v>0.17316666666666666</v>
+      </c>
+      <c r="G5" s="23">
+        <f t="shared" si="1"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>0.43</v>
+      </c>
+      <c r="B6" s="2">
+        <v>4480</v>
+      </c>
+      <c r="C6" s="2">
+        <v>372</v>
+      </c>
+      <c r="D6" s="2">
+        <v>665</v>
+      </c>
+      <c r="E6" s="2">
+        <v>483</v>
+      </c>
+      <c r="F6" s="24">
+        <f t="shared" si="0"/>
+        <v>0.17283333333333334</v>
+      </c>
+      <c r="G6" s="23">
+        <f t="shared" si="1"/>
+        <v>8.0500000000000002E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>0.44</v>
+      </c>
+      <c r="B7" s="2">
+        <v>4503</v>
+      </c>
+      <c r="C7" s="2">
+        <v>349</v>
+      </c>
+      <c r="D7" s="2">
+        <v>679</v>
+      </c>
+      <c r="E7" s="2">
+        <v>469</v>
+      </c>
+      <c r="F7" s="24">
+        <f t="shared" si="0"/>
+        <v>0.17133333333333334</v>
+      </c>
+      <c r="G7" s="23">
+        <f t="shared" si="1"/>
+        <v>7.8166666666666662E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
         <v>0.45</v>
       </c>
-      <c r="B3" s="7">
-        <v>4564</v>
-      </c>
-      <c r="C3" s="7">
-        <v>288</v>
-      </c>
-      <c r="D3" s="7">
-        <v>753</v>
-      </c>
-      <c r="E3" s="7">
-        <v>395</v>
-      </c>
-      <c r="F3" s="11">
-        <f>(C3+D3)/SUM(B3:E3)</f>
-        <v>0.17349999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
+      <c r="B8" s="2">
+        <v>4521</v>
+      </c>
+      <c r="C8" s="2">
+        <v>331</v>
+      </c>
+      <c r="D8" s="2">
+        <v>693</v>
+      </c>
+      <c r="E8" s="2">
+        <v>455</v>
+      </c>
+      <c r="F8" s="24">
+        <f t="shared" si="0"/>
+        <v>0.17066666666666666</v>
+      </c>
+      <c r="G8" s="23">
+        <f t="shared" si="1"/>
+        <v>7.5833333333333336E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
         <v>0.46</v>
       </c>
-      <c r="B4" s="7">
-        <v>4585</v>
-      </c>
-      <c r="C4" s="7">
-        <v>267</v>
-      </c>
-      <c r="D4" s="7">
-        <v>766</v>
-      </c>
-      <c r="E4" s="7">
-        <v>382</v>
-      </c>
-      <c r="F4" s="11">
-        <f t="shared" ref="F4:F13" si="0">(C4+D4)/SUM(B4:E4)</f>
-        <v>0.17216666666666666</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
+      <c r="B9" s="2">
+        <v>4540</v>
+      </c>
+      <c r="C9" s="2">
+        <v>312</v>
+      </c>
+      <c r="D9" s="2">
+        <v>717</v>
+      </c>
+      <c r="E9" s="2">
+        <v>431</v>
+      </c>
+      <c r="F9" s="24">
+        <f t="shared" si="0"/>
+        <v>0.17150000000000001</v>
+      </c>
+      <c r="G9" s="23">
+        <f t="shared" si="1"/>
+        <v>7.1833333333333332E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
         <v>0.47</v>
       </c>
-      <c r="B5" s="7">
-        <v>4597</v>
-      </c>
-      <c r="C5" s="7">
-        <v>255</v>
-      </c>
-      <c r="D5" s="7">
-        <v>777</v>
-      </c>
-      <c r="E5" s="7">
-        <v>371</v>
-      </c>
-      <c r="F5" s="11">
+      <c r="B10" s="2">
+        <v>4561</v>
+      </c>
+      <c r="C10" s="2">
+        <v>291</v>
+      </c>
+      <c r="D10" s="2">
+        <v>740</v>
+      </c>
+      <c r="E10" s="2">
+        <v>408</v>
+      </c>
+      <c r="F10" s="24">
+        <f t="shared" si="0"/>
+        <v>0.17183333333333334</v>
+      </c>
+      <c r="G10" s="23">
+        <f t="shared" si="1"/>
+        <v>6.8000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>0.48</v>
+      </c>
+      <c r="B11" s="2">
+        <v>4580</v>
+      </c>
+      <c r="C11" s="2">
+        <v>272</v>
+      </c>
+      <c r="D11" s="2">
+        <v>760</v>
+      </c>
+      <c r="E11" s="2">
+        <v>388</v>
+      </c>
+      <c r="F11" s="24">
         <f t="shared" si="0"/>
         <v>0.17199999999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
-        <v>0.48</v>
-      </c>
-      <c r="B6" s="7">
-        <v>4616</v>
-      </c>
-      <c r="C6" s="7">
-        <v>236</v>
-      </c>
-      <c r="D6" s="7">
-        <v>788</v>
-      </c>
-      <c r="E6" s="7">
-        <v>360</v>
-      </c>
-      <c r="F6" s="11">
-        <f t="shared" si="0"/>
-        <v>0.17066666666666666</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
+      <c r="G11" s="23">
+        <f t="shared" si="1"/>
+        <v>6.4666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
         <v>0.49</v>
       </c>
-      <c r="B7" s="7">
-        <v>4636</v>
-      </c>
-      <c r="C7" s="7">
-        <v>216</v>
-      </c>
-      <c r="D7" s="7">
-        <v>806</v>
-      </c>
-      <c r="E7" s="7">
-        <v>342</v>
-      </c>
-      <c r="F7" s="11">
-        <f t="shared" si="0"/>
-        <v>0.17033333333333334</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
+      <c r="B12" s="2">
+        <v>4600</v>
+      </c>
+      <c r="C12" s="2">
+        <v>252</v>
+      </c>
+      <c r="D12" s="2">
+        <v>771</v>
+      </c>
+      <c r="E12" s="2">
+        <v>377</v>
+      </c>
+      <c r="F12" s="24">
+        <f t="shared" si="0"/>
+        <v>0.17050000000000001</v>
+      </c>
+      <c r="G12" s="23">
+        <f t="shared" si="1"/>
+        <v>6.2833333333333338E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
         <v>0.5</v>
       </c>
-      <c r="B8" s="7">
-        <v>4651</v>
-      </c>
-      <c r="C8" s="7">
-        <v>201</v>
-      </c>
-      <c r="D8" s="7">
-        <v>819</v>
-      </c>
-      <c r="E8" s="7">
-        <v>329</v>
-      </c>
-      <c r="F8" s="11">
+      <c r="B13" s="2">
+        <v>4617</v>
+      </c>
+      <c r="C13" s="2">
+        <v>235</v>
+      </c>
+      <c r="D13" s="2">
+        <v>785</v>
+      </c>
+      <c r="E13" s="2">
+        <v>363</v>
+      </c>
+      <c r="F13" s="24">
         <f t="shared" si="0"/>
         <v>0.17</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
-        <v>0.51</v>
-      </c>
-      <c r="B9" s="7">
-        <v>4664</v>
-      </c>
-      <c r="C9" s="7">
-        <v>188</v>
-      </c>
-      <c r="D9" s="7">
-        <v>833</v>
-      </c>
-      <c r="E9" s="7">
-        <v>315</v>
-      </c>
-      <c r="F9" s="11">
-        <f t="shared" si="0"/>
-        <v>0.17016666666666666</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
-        <v>0.52</v>
-      </c>
-      <c r="B10" s="7">
-        <v>4675</v>
-      </c>
-      <c r="C10" s="7">
-        <v>177</v>
-      </c>
-      <c r="D10" s="7">
-        <v>851</v>
-      </c>
-      <c r="E10" s="7">
-        <v>297</v>
-      </c>
-      <c r="F10" s="11">
-        <f t="shared" si="0"/>
-        <v>0.17133333333333334</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
-        <v>0.53</v>
-      </c>
-      <c r="B11" s="7">
-        <v>4690</v>
-      </c>
-      <c r="C11" s="7">
-        <v>162</v>
-      </c>
-      <c r="D11" s="7">
-        <v>873</v>
-      </c>
-      <c r="E11" s="7">
-        <v>275</v>
-      </c>
-      <c r="F11" s="11">
-        <f t="shared" si="0"/>
-        <v>0.17249999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
-        <v>0.54</v>
-      </c>
-      <c r="B12" s="7">
-        <v>4704</v>
-      </c>
-      <c r="C12" s="7">
-        <v>148</v>
-      </c>
-      <c r="D12" s="7">
-        <v>890</v>
-      </c>
-      <c r="E12" s="7">
-        <v>258</v>
-      </c>
-      <c r="F12" s="11">
-        <f t="shared" si="0"/>
-        <v>0.17299999999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="B13" s="7">
-        <v>4718</v>
-      </c>
-      <c r="C13" s="7">
-        <v>134</v>
-      </c>
-      <c r="D13" s="7">
-        <v>902</v>
-      </c>
-      <c r="E13" s="7">
-        <v>246</v>
-      </c>
-      <c r="F13" s="11">
-        <f t="shared" si="0"/>
-        <v>0.17266666666666666</v>
+      <c r="G13" s="23">
+        <f t="shared" si="1"/>
+        <v>6.0499999999999998E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>0.50999999999999901</v>
+      </c>
+      <c r="F14" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>0.51999999999999902</v>
+      </c>
+      <c r="F15" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>0.52999999999999903</v>
+      </c>
+      <c r="F16" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>0.53999999999999904</v>
+      </c>
+      <c r="F17" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>0.54999999999999905</v>
+      </c>
+      <c r="F18" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>0.55999999999999905</v>
+      </c>
+      <c r="F19" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>0.56999999999999895</v>
+      </c>
+      <c r="F20" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <v>0.57999999999999896</v>
+      </c>
+      <c r="F21" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>0.58999999999999897</v>
+      </c>
+      <c r="F22" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>0.59999999999999898</v>
+      </c>
+      <c r="F23" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>